<commit_message>
Modularization of the proyect
</commit_message>
<xml_diff>
--- a/7 Palabras .xlsx
+++ b/7 Palabras .xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>Actividad A</t>
   </si>
@@ -74,38 +74,50 @@
     <t>Comprender el funcionamiento del algoritmo Isolation Forest</t>
   </si>
   <si>
+    <t>Apagon</t>
+  </si>
+  <si>
+    <t>"Estudiar Kali en Profundidad"</t>
+  </si>
+  <si>
+    <t>Mejorar el PPT de Metodología</t>
+  </si>
+  <si>
+    <t>Base de datos de la problemática</t>
+  </si>
+  <si>
+    <t>Modularizar el software</t>
+  </si>
+  <si>
     <t>Ver como realizar un mejor preprocesamiento de los datos</t>
   </si>
   <si>
-    <t>Mejorar el PPT de Metodología</t>
-  </si>
-  <si>
-    <t>ChatGPT con el tema de Alex y el mio</t>
-  </si>
-  <si>
-    <t>Estudiar Kali en Profundidad</t>
+    <t>Ver como añadir mas algoritmos y su eficiencia</t>
   </si>
   <si>
     <t>Arreglar el acceso a la base de datos sql segun la consulta</t>
   </si>
   <si>
     <t>Metodología de la Investigación relacionados con su TESIS</t>
-  </si>
-  <si>
-    <t>Hacer que un chatbot te explique el analisis de los datos</t>
   </si>
   <si>
     <t>Base de datos de las
   5 referencias bibliográficas que le reflejan la situación problemática</t>
   </si>
   <si>
+    <t>ChatGPT con el tema de Alex y el mio</t>
+  </si>
+  <si>
     <t>Revisar Introducción y entregar al tutor</t>
   </si>
   <si>
     <t>Entregar al tutor Capítulo 1 para revisión</t>
   </si>
   <si>
-    <t>Rectificar Introducción y Capítulo 1</t>
+    <t>Estudiar Kali en Profundidad</t>
+  </si>
+  <si>
+    <t>Hacer que un chatbot te explique el analisis de los datos</t>
   </si>
   <si>
     <t>Entregar Introducción y Capítulo 1 rectificado</t>
@@ -149,7 +161,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +184,13 @@
     </font>
     <font>
       <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -640,137 +659,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,6 +811,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1118,8 +1143,8 @@
   <sheetPr/>
   <dimension ref="A1:D261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1213,196 +1238,240 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="6">
         <v>45583</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D7" s="6">
         <v>45584</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D8" s="6">
         <v>45585</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
+      <c r="A9" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D9" s="6">
         <v>45586</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
+      <c r="A10" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D10" s="6">
         <v>45587</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
+      <c r="A11" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D11" s="6">
         <v>45588</v>
       </c>
     </row>
-    <row r="12" ht="27.6" spans="1:4">
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D12" s="6">
         <v>45589</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="6">
         <v>45590</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="D14" s="6">
         <v>45591</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D15" s="6">
         <v>45592</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+    <row r="16" ht="41.4" spans="1:4">
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="D16" s="6">
         <v>45593</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D17" s="6">
         <v>45594</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D18" s="6">
         <v>45595</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+    <row r="19" spans="3:4">
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D19" s="6">
         <v>45596</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+    <row r="20" spans="2:4">
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D20" s="6">
         <v>45597</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D21" s="6">
         <v>45598</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D22" s="6">
         <v>45599</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+    <row r="23" spans="2:4">
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D23" s="6">
         <v>45600</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+    <row r="24" spans="3:4">
       <c r="C24" s="2"/>
       <c r="D24" s="6">
         <v>45601</v>
@@ -1410,7 +1479,9 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="6">
         <v>45602</v>
@@ -1424,126 +1495,79 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2"/>
+    <row r="27" spans="2:4">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="6">
         <v>45604</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+    <row r="28" spans="4:4">
       <c r="D28" s="6">
         <v>45605</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+    <row r="29" spans="4:4">
       <c r="D29" s="6">
         <v>45606</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+    <row r="30" spans="4:4">
       <c r="D30" s="6">
         <v>45607</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+    <row r="31" spans="4:4">
       <c r="D31" s="6">
         <v>45608</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+    <row r="32" spans="4:4">
       <c r="D32" s="6">
         <v>45609</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+    <row r="33" spans="4:4">
       <c r="D33" s="6">
         <v>45610</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+    <row r="34" spans="4:4">
       <c r="D34" s="6">
         <v>45611</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+    <row r="35" spans="4:4">
       <c r="D35" s="6">
         <v>45612</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+    <row r="36" spans="4:4">
       <c r="D36" s="6">
         <v>45613</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+    <row r="37" spans="4:4">
       <c r="D37" s="6">
         <v>45614</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+    <row r="38" spans="4:4">
       <c r="D38" s="6">
         <v>45615</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+    <row r="39" spans="4:4">
       <c r="D39" s="6">
         <v>45616</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+    <row r="40" spans="4:4">
       <c r="D40" s="6">
         <v>45617</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+    <row r="41" spans="4:4">
       <c r="D41" s="6">
         <v>45618</v>
       </c>
@@ -1582,7 +1606,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1608,7 +1632,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1649,7 +1673,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1691,7 +1715,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1723,8 +1747,8 @@
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="9" t="s">
-        <v>30</v>
+      <c r="A63" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1750,7 +1774,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1783,7 +1807,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="6">
@@ -1840,7 +1864,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1898,7 +1922,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3316,7 +3340,7 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>

</xml_diff>